<commit_message>
Update burndown for sprint 2
</commit_message>
<xml_diff>
--- a/API Project Sprint Planning.xlsx
+++ b/API Project Sprint Planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterzorzonello/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterzorzonello/Documents/GitHub/BU_API_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB44576-E8F3-5648-9E22-8363B7BB94D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF48782-5F46-A648-91DE-66840623CFB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,6 @@
     <sheet name="Sprint 3 Burndown" sheetId="5" r:id="rId6"/>
     <sheet name="Sprint 4 Burndown" sheetId="6" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sprint 2 Burndown'!$B$14:$E$14</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sprint 2 Burndown'!$B$15:$E$15</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sprint 2 Burndown'!$B$7:$E$7</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -817,7 +812,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3245,7 +3240,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3289,6 +3284,9 @@
       <c r="B8">
         <v>4</v>
       </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -3297,6 +3295,9 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -3305,6 +3306,9 @@
       <c r="B10">
         <v>2</v>
       </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -3313,6 +3317,9 @@
       <c r="B11">
         <v>4</v>
       </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -3321,6 +3328,9 @@
       <c r="B12">
         <v>4</v>
       </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -3332,7 +3342,7 @@
       </c>
       <c r="C14">
         <f>SUM(C8:C12)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <f>SUM(D8:D12)</f>

</xml_diff>

<commit_message>
Updated with 9/11/18's work
updated burndown late for 9/11
</commit_message>
<xml_diff>
--- a/API Project Sprint Planning.xlsx
+++ b/API Project Sprint Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterzorzonello/Documents/GitHub/BU_API_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF48782-5F46-A648-91DE-66840623CFB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006FFDF0-C936-764B-BB41-D4E9F80F05F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -815,7 +815,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2699,12 +2699,12 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2885,12 +2885,12 @@
       <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2969,13 +2969,13 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2986,12 +2986,12 @@
         <v>43352</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3011,7 +3011,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3168,12 +3168,12 @@
       <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -3239,17 +3239,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>43355</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>43355</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3287,8 +3287,11 @@
       <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3298,8 +3301,11 @@
       <c r="C9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3309,8 +3315,11 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3320,8 +3329,11 @@
       <c r="C11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -3331,8 +3343,11 @@
       <c r="C12">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3346,14 +3361,14 @@
       </c>
       <c r="D14">
         <f>SUM(D8:D12)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E14">
         <f>SUM(E8:E12)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3385,13 +3400,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3402,7 +3417,7 @@
         <v>43358</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3432,13 +3447,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3449,7 +3464,7 @@
         <v>43361</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Close Sprint 2, Start Sprint 3
</commit_message>
<xml_diff>
--- a/API Project Sprint Planning.xlsx
+++ b/API Project Sprint Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterzorzonello/Documents/GitHub/BU_API_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A21109-144C-EE44-BE13-026CE446C4BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05680900-E198-4A41-B2AF-99E3EC6148F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,11 @@
     <sheet name="Sprint 3 Burndown" sheetId="5" r:id="rId6"/>
     <sheet name="Sprint 4 Burndown" sheetId="6" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Sprint 3 Burndown'!$B$13:$E$13</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Sprint 3 Burndown'!$B$14:$E$14</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Sprint 3 Burndown'!$B$7:$E$7</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t xml:space="preserve">Stories </t>
   </si>
@@ -818,7 +823,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1175,6 +1180,486 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>BurnDown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Burndown</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0.5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3 Burndown'!$B$13:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-95B9-4141-9AFE-B467AD9772F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-148918176"/>
+        <c:axId val="-97462208"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Desired Burndown</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 3 Burndown'!$B$7:$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Starting  Hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9/13/18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9/14/18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9/15/18</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3 Burndown'!$B$14:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3333333333333326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-95B9-4141-9AFE-B467AD9772F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-148918176"/>
+        <c:axId val="-97462208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-148918176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-97462208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-97462208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-148918176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1255,6 +1740,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1772,6 +2297,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2349,6 +3390,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51C2F1BC-55C2-454F-A25C-F178709A4BD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>437602</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>129510</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F15E468E-32A9-914D-BAB6-D6C505FACA2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2696,7 +3780,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2735,11 +3819,14 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2776,26 +3863,35 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>4</v>
       </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>4</v>
       </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3239,8 +4335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3359,7 +4455,7 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3380,7 +4476,7 @@
       </c>
       <c r="E14">
         <f>SUM(E8:E12)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3411,13 +4507,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3449,8 +4547,94 @@
         <v>43358</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B8:B11)</f>
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f>SUM(C8:C11)</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f>SUM(D8:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <f>B13</f>
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <f>B13-(B13/3)</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="D14">
+        <f>C14-(B13/3)</f>
+        <v>3.3333333333333326</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update the Sprint Planning
</commit_message>
<xml_diff>
--- a/API Project Sprint Planning.xlsx
+++ b/API Project Sprint Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterzorzonello/Documents/GitHub/BU_API_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22A01D9-4F6E-D644-A1D5-EBB60274D3A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1170FCC-BB31-3E42-BC01-CEE9786C8540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1805,10 +1805,10 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -5631,8 +5631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5788,8 +5788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5833,6 +5833,12 @@
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -5841,6 +5847,12 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -5849,6 +5861,12 @@
       <c r="B10">
         <v>2</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5857,6 +5875,12 @@
       <c r="B11">
         <v>2</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -5865,6 +5889,12 @@
       <c r="B12">
         <v>2</v>
       </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -5876,11 +5906,11 @@
       </c>
       <c r="C14">
         <f>SUM(C8:C12)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <f>SUM(D8:D12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <f>SUM(E8:E12)</f>

</xml_diff>